<commit_message>
Added VWA charts and columns
</commit_message>
<xml_diff>
--- a/data/YIELD_LT.xlsx
+++ b/data/YIELD_LT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevineriksson/PycharmProjects/Simulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16ADD779-AE65-F649-B030-1E61603822E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FEBCDE-3378-F040-BB7C-15FFB78DC595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8340" yWindow="2400" windowWidth="27240" windowHeight="13760" xr2:uid="{B2249A4F-5109-C145-A437-E2DC31518187}"/>
+    <workbookView xWindow="11160" yWindow="560" windowWidth="27240" windowHeight="13760" xr2:uid="{B2249A4F-5109-C145-A437-E2DC31518187}"/>
   </bookViews>
   <sheets>
     <sheet name="Yearly" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>SOLAR - Annual prod MWh, MW</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>installed power</t>
   </si>
 </sst>
 </file>
@@ -98,12 +101,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515D34A8-24E4-3341-8497-6EDB0F5D2285}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -452,7 +456,7 @@
     <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -462,80 +466,125 @@
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>2020</v>
       </c>
-      <c r="B2">
-        <v>3500</v>
+      <c r="B2" s="4">
+        <v>2788.2166666666667</v>
       </c>
       <c r="C2" s="3">
         <v>451.90243902439022</v>
       </c>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>2020</v>
+      </c>
+      <c r="H2">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2021</v>
       </c>
-      <c r="B3" s="3">
-        <v>2345.9988629496347</v>
+      <c r="B3" s="4">
+        <v>1868.9008941877794</v>
       </c>
       <c r="C3" s="3">
         <v>495.74509803921569</v>
       </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>2021</v>
+      </c>
+      <c r="H3">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2022</v>
       </c>
-      <c r="B4" s="3">
-        <v>1958.7312339003788</v>
+      <c r="B4" s="4">
+        <v>2079.0556338028168</v>
       </c>
       <c r="C4" s="3">
         <v>614.95804195804192</v>
       </c>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>2022</v>
+      </c>
+      <c r="H4">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2023</v>
       </c>
-      <c r="B5" s="3">
-        <v>2502.8143409253425</v>
+      <c r="B5" s="4">
+        <v>2408.5410000000002</v>
       </c>
       <c r="C5" s="3">
         <v>562.0987124463519</v>
       </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>2023</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>2024</v>
       </c>
-      <c r="B6" s="3">
-        <v>2360.5550739600553</v>
+      <c r="B6" s="4">
+        <v>2531.4380768461538</v>
       </c>
       <c r="C6" s="3">
         <v>542.79262434748728</v>
       </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F6" s="5"/>
+      <c r="G6">
+        <v>2024</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>